<commit_message>
Final Compile for Fall 2020 Class
I made numerous tweaks to the book while creating help videos for the students. This is the final compile before the Fall 2020 class.
</commit_message>
<xml_diff>
--- a/Student Files/CH4-Charting Solution 1_1.xlsx
+++ b/Student Files/CH4-Charting Solution 1_1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gself\Desktop\Excel 365 Exercises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gself\Dropbox\GitHub\cll_excel\Student Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A545646-F9AF-4EFF-BC5B-53AEAF74C125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0C5681-23C1-4C51-A5AF-C8550F623FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="675" windowWidth="19365" windowHeight="14205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30525" yWindow="645" windowWidth="16485" windowHeight="14340" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Closing Prices" sheetId="5" r:id="rId1"/>
     <sheet name="Stock Trend" sheetId="2" r:id="rId2"/>
     <sheet name="All Excel Classes" sheetId="6" r:id="rId3"/>
     <sheet name="Grade Distribution" sheetId="1" r:id="rId4"/>
-    <sheet name="Enrolment Statistics" sheetId="3" r:id="rId5"/>
+    <sheet name="Enrollment Statistics" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -1991,6 +1991,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="611965360"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2886,7 +2887,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$B$2</c:f>
+              <c:f>'Enrollment Statistics'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2910,6 +2911,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-15B9-41DC-9C72-7D7F70C114CB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2925,6 +2931,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-15B9-41DC-9C72-7D7F70C114CB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2940,6 +2951,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-15B9-41DC-9C72-7D7F70C114CB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2955,6 +2971,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-15B9-41DC-9C72-7D7F70C114CB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3013,7 +3034,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$A$3:$A$6</c:f>
+              <c:f>'Enrollment Statistics'!$A$3:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3033,7 +3054,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Enrolment Statistics'!$B$3:$B$6</c:f>
+              <c:f>'Enrollment Statistics'!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3202,7 +3223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$A$3</c:f>
+              <c:f>'Enrollment Statistics'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3223,7 +3244,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$B$2:$D$2</c:f>
+              <c:f>'Enrollment Statistics'!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3240,7 +3261,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Enrolment Statistics'!$B$3:$D$3</c:f>
+              <c:f>'Enrollment Statistics'!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3267,7 +3288,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$A$4</c:f>
+              <c:f>'Enrollment Statistics'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3288,7 +3309,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$B$2:$D$2</c:f>
+              <c:f>'Enrollment Statistics'!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3305,7 +3326,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Enrolment Statistics'!$B$4:$D$4</c:f>
+              <c:f>'Enrollment Statistics'!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3332,7 +3353,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$A$5</c:f>
+              <c:f>'Enrollment Statistics'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3353,7 +3374,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$B$2:$D$2</c:f>
+              <c:f>'Enrollment Statistics'!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3370,7 +3391,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Enrolment Statistics'!$B$5:$D$5</c:f>
+              <c:f>'Enrollment Statistics'!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3397,7 +3418,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$A$6</c:f>
+              <c:f>'Enrollment Statistics'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3418,7 +3439,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Enrolment Statistics'!$B$2:$D$2</c:f>
+              <c:f>'Enrollment Statistics'!$B$2:$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3435,7 +3456,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Enrolment Statistics'!$B$6:$D$6</c:f>
+              <c:f>'Enrollment Statistics'!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -8119,7 +8140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
@@ -9240,7 +9261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>